<commit_message>
(feat):reading student id and student name from backend to front end
</commit_message>
<xml_diff>
--- a/student_timetable/1234_timetable.xlsx
+++ b/student_timetable/1234_timetable.xlsx
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="D11" s="6" t="n">
-        <v>2222</v>
+        <v>3233</v>
       </c>
       <c r="E11" s="6" t="n">
         <v/>
@@ -681,21 +681,21 @@
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>7:00 to 8:00(L + T)</t>
+          <t>12:00 to 13:00(L + T)</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>MITS5501-(1h Lecture 2)</t>
+          <t>MITS5501-(1h Tutorial 1)</t>
         </is>
       </c>
       <c r="D12" s="6" t="n">
-        <v>6666</v>
+        <v>4321</v>
       </c>
       <c r="E12" s="6" t="n">
         <v/>
@@ -717,16 +717,16 @@
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>12:00 to 13:00(L + T)</t>
+          <t>7:00 to 8:00(L + T)</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>MITS5502-(1h Lab 1)</t>
+          <t>MITS5501-(1h Lecture 2)</t>
         </is>
       </c>
       <c r="D13" s="6" t="n">
-        <v>321</v>
+        <v>6666</v>
       </c>
       <c r="E13" s="6" t="n">
         <v/>
@@ -748,16 +748,16 @@
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
-          <t>20:00 to 21:00(L + T)</t>
+          <t>14:00 to 15:00(L + T)</t>
         </is>
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>MITS5502-(1h Lecture 1)</t>
+          <t>MITS5502-(1h Lab 1)</t>
         </is>
       </c>
       <c r="D14" s="6" t="n">
-        <v>432</v>
+        <v>4321</v>
       </c>
       <c r="E14" s="6" t="n">
         <v/>
@@ -767,28 +767,28 @@
       </c>
       <c r="G14" s="6" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>oncampus</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>10:00 to 11:00(L + T)</t>
+          <t>20:00 to 21:00(L + T)</t>
         </is>
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>MITS5501-(1h Lab 1)</t>
+          <t>MITS5502-(1h Lecture 1)</t>
         </is>
       </c>
       <c r="D15" s="6" t="n">
-        <v>4321</v>
+        <v>432</v>
       </c>
       <c r="E15" s="6" t="n">
         <v/>
@@ -798,7 +798,7 @@
       </c>
       <c r="G15" s="6" t="inlineStr">
         <is>
-          <t>oncampus</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -810,12 +810,12 @@
       </c>
       <c r="B16" s="6" t="inlineStr">
         <is>
-          <t>12:00 to 13:00(L + T)</t>
+          <t>10:00 to 11:00(L + T)</t>
         </is>
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>MITS5501-(1h Tutorial 1)</t>
+          <t>MITS5501-(1h Lab 1)</t>
         </is>
       </c>
       <c r="D16" s="6" t="n">

</xml_diff>